<commit_message>
men data updated - sheet total everywhere
</commit_message>
<xml_diff>
--- a/data/men/M_2018_12_Memorial.xlsx
+++ b/data/men/M_2018_12_Memorial.xlsx
@@ -8,26 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\data\men\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C5F035-648C-411D-9D1B-A3EEF1BEC0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08817500-F0E3-463F-B6B1-E8EECC8B6421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="-16392" windowWidth="17376" windowHeight="15192" tabRatio="670" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="-16632" windowWidth="25488" windowHeight="10380" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="initiation" sheetId="1" r:id="rId1"/>
-    <sheet name="first_round" sheetId="2" r:id="rId2"/>
-    <sheet name="total_rank" sheetId="3" r:id="rId3"/>
-    <sheet name="pools" sheetId="4" r:id="rId4"/>
-    <sheet name="eliminations" sheetId="5" r:id="rId5"/>
+    <sheet name="total" sheetId="6" r:id="rId1"/>
+    <sheet name="initiation" sheetId="1" r:id="rId2"/>
+    <sheet name="first_round" sheetId="2" r:id="rId3"/>
+    <sheet name="total_rank" sheetId="3" r:id="rId4"/>
+    <sheet name="pools" sheetId="4" r:id="rId5"/>
+    <sheet name="eliminations" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">eliminations!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">first_round!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initiation!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pools!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">total_rank!$A$1:$H$1</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">first_round!#REF!</definedName>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">initiation!#REF!</definedName>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">total_rank!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">eliminations!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">first_round!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">initiation!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">pools!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">total_rank!$A$1:$H$1</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">first_round!#REF!</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">initiation!#REF!</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">total_rank!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7489" uniqueCount="143">
   <si>
     <t>Name</t>
   </si>
@@ -477,6 +479,9 @@
   <si>
     <t>Eliminace_128</t>
   </si>
+  <si>
+    <t>Percentil</t>
+  </si>
 </sst>
 </file>
 
@@ -562,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -608,6 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,11 +893,4336 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168B5695-45C2-4A05-A24D-A3D77E87F1FE}">
+  <dimension ref="A1:Q83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="21">
+        <v>26542</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K2" s="19">
+        <v>26</v>
+      </c>
+      <c r="L2">
+        <f>K2-M2</f>
+        <v>31</v>
+      </c>
+      <c r="M2" s="19">
+        <v>-5</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="19">
+        <v>59</v>
+      </c>
+      <c r="P2" s="22">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="31">
+        <f>P2/MAX($P$2:$P$81)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="21">
+        <v>28313</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K3">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <f>K3-M3</f>
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>-7</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3">
+        <v>69</v>
+      </c>
+      <c r="P3" s="22">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="31">
+        <f t="shared" ref="Q3:Q66" si="0">P3/MAX($P$2:$P$81)</f>
+        <v>0.76249999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="21">
+        <v>36099</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K4" s="19">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <f>K4-M4</f>
+        <v>17</v>
+      </c>
+      <c r="M4" s="19">
+        <v>14</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="19">
+        <v>10</v>
+      </c>
+      <c r="P4" s="22">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="31">
+        <f t="shared" si="0"/>
+        <v>0.13750000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="1">
+        <v>35522</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K5" s="19">
+        <v>17</v>
+      </c>
+      <c r="L5">
+        <f>K5-M5</f>
+        <v>29</v>
+      </c>
+      <c r="M5" s="19">
+        <v>-12</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="19">
+        <v>66</v>
+      </c>
+      <c r="P5">
+        <v>71</v>
+      </c>
+      <c r="Q5" s="31">
+        <f t="shared" si="0"/>
+        <v>0.88749999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="21">
+        <v>37753</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="22">
+        <v>0</v>
+      </c>
+      <c r="K6" s="22">
+        <v>14</v>
+      </c>
+      <c r="L6">
+        <f>K6-M6</f>
+        <v>35</v>
+      </c>
+      <c r="M6" s="22">
+        <v>-21</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="22">
+        <v>75</v>
+      </c>
+      <c r="P6" s="22">
+        <v>64</v>
+      </c>
+      <c r="Q6" s="31">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="21">
+        <v>29969</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7" s="19">
+        <v>1</v>
+      </c>
+      <c r="K7" s="19">
+        <v>35</v>
+      </c>
+      <c r="L7">
+        <f>K7-M7</f>
+        <v>18</v>
+      </c>
+      <c r="M7" s="19">
+        <v>17</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="19">
+        <v>4</v>
+      </c>
+      <c r="P7" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="31">
+        <f t="shared" si="0"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="21">
+        <v>34040</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K8" s="19">
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <f>K8-M8</f>
+        <v>13</v>
+      </c>
+      <c r="M8" s="19">
+        <v>17</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="19">
+        <v>12</v>
+      </c>
+      <c r="P8" s="22">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="31">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="21">
+        <v>19450</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="22">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K9" s="22">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <f>K9-M9</f>
+        <v>34</v>
+      </c>
+      <c r="M9" s="22">
+        <v>-26</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="22">
+        <v>74</v>
+      </c>
+      <c r="P9" s="22">
+        <v>63</v>
+      </c>
+      <c r="Q9" s="31">
+        <f t="shared" si="0"/>
+        <v>0.78749999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="21">
+        <v>35185</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K10" s="19">
+        <v>28</v>
+      </c>
+      <c r="L10">
+        <f>K10-M10</f>
+        <v>29</v>
+      </c>
+      <c r="M10" s="19">
+        <v>-1</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="19">
+        <v>45</v>
+      </c>
+      <c r="P10" s="22">
+        <v>47</v>
+      </c>
+      <c r="Q10" s="31">
+        <f t="shared" si="0"/>
+        <v>0.58750000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="21">
+        <v>37031</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K11" s="19">
+        <v>27</v>
+      </c>
+      <c r="L11">
+        <f>K11-M11</f>
+        <v>26</v>
+      </c>
+      <c r="M11" s="19">
+        <v>1</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="19">
+        <v>43</v>
+      </c>
+      <c r="P11" s="22">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="31">
+        <f t="shared" si="0"/>
+        <v>0.38750000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="1">
+        <v>30117</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K12" s="19">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <f>K12-M12</f>
+        <v>30</v>
+      </c>
+      <c r="M12" s="19">
+        <v>-10</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="19">
+        <v>64</v>
+      </c>
+      <c r="P12">
+        <v>70</v>
+      </c>
+      <c r="Q12" s="31">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="21">
+        <v>37662</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K13" s="19">
+        <v>32</v>
+      </c>
+      <c r="L13">
+        <f>K13-M13</f>
+        <v>19</v>
+      </c>
+      <c r="M13" s="19">
+        <v>13</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="19">
+        <v>27</v>
+      </c>
+      <c r="P13" s="22">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="31">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="21">
+        <v>30573</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14" s="19">
+        <v>1</v>
+      </c>
+      <c r="K14" s="19">
+        <v>35</v>
+      </c>
+      <c r="L14">
+        <f>K14-M14</f>
+        <v>10</v>
+      </c>
+      <c r="M14" s="19">
+        <v>25</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="19">
+        <v>2</v>
+      </c>
+      <c r="P14" s="22">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="31">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="21">
+        <v>33595</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K15" s="19">
+        <v>32</v>
+      </c>
+      <c r="L15">
+        <f>K15-M15</f>
+        <v>13</v>
+      </c>
+      <c r="M15" s="19">
+        <v>19</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="19">
+        <v>6</v>
+      </c>
+      <c r="P15" s="22">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="31">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="21">
+        <v>35542</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K16" s="19">
+        <v>30</v>
+      </c>
+      <c r="L16">
+        <f>K16-M16</f>
+        <v>20</v>
+      </c>
+      <c r="M16" s="19">
+        <v>10</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="19">
+        <v>11</v>
+      </c>
+      <c r="P16" s="22">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="31">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="21">
+        <v>34315</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K17" s="19">
+        <v>31</v>
+      </c>
+      <c r="L17">
+        <f>K17-M17</f>
+        <v>23</v>
+      </c>
+      <c r="M17" s="19">
+        <v>8</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="19">
+        <v>22</v>
+      </c>
+      <c r="P17" s="22">
+        <v>35</v>
+      </c>
+      <c r="Q17" s="31">
+        <f t="shared" si="0"/>
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="21">
+        <v>35667</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K18" s="19">
+        <v>29</v>
+      </c>
+      <c r="L18">
+        <f>K18-M18</f>
+        <v>19</v>
+      </c>
+      <c r="M18" s="19">
+        <v>10</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="19">
+        <v>19</v>
+      </c>
+      <c r="P18" s="22">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="31">
+        <f t="shared" si="0"/>
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="21">
+        <v>34757</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="22">
+        <v>0</v>
+      </c>
+      <c r="K19" s="22">
+        <v>11</v>
+      </c>
+      <c r="L19">
+        <f>K19-M19</f>
+        <v>35</v>
+      </c>
+      <c r="M19" s="22">
+        <v>-24</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="22">
+        <v>78</v>
+      </c>
+      <c r="P19" s="22">
+        <v>78</v>
+      </c>
+      <c r="Q19" s="31">
+        <f t="shared" si="0"/>
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="21">
+        <v>36046</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K20" s="19">
+        <v>26</v>
+      </c>
+      <c r="L20">
+        <f>K20-M20</f>
+        <v>26</v>
+      </c>
+      <c r="M20" s="19">
+        <v>0</v>
+      </c>
+      <c r="N20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" s="19">
+        <v>38</v>
+      </c>
+      <c r="P20" s="22">
+        <v>42</v>
+      </c>
+      <c r="Q20" s="31">
+        <f t="shared" si="0"/>
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="21">
+        <v>31413</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K21" s="19">
+        <v>24</v>
+      </c>
+      <c r="L21">
+        <f>K21-M21</f>
+        <v>24</v>
+      </c>
+      <c r="M21" s="19">
+        <v>0</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="19">
+        <v>39</v>
+      </c>
+      <c r="P21" s="22">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="31">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="21">
+        <v>34286</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K22" s="19">
+        <v>24</v>
+      </c>
+      <c r="L22">
+        <f>K22-M22</f>
+        <v>30</v>
+      </c>
+      <c r="M22" s="19">
+        <v>-6</v>
+      </c>
+      <c r="N22" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="19">
+        <v>52</v>
+      </c>
+      <c r="P22" s="22">
+        <v>52</v>
+      </c>
+      <c r="Q22" s="31">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="21">
+        <v>33673</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+      <c r="J23" s="19">
+        <v>1</v>
+      </c>
+      <c r="K23" s="19">
+        <v>35</v>
+      </c>
+      <c r="L23">
+        <f>K23-M23</f>
+        <v>19</v>
+      </c>
+      <c r="M23" s="19">
+        <v>16</v>
+      </c>
+      <c r="N23" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="19">
+        <v>5</v>
+      </c>
+      <c r="P23" s="22">
+        <v>9</v>
+      </c>
+      <c r="Q23" s="31">
+        <f t="shared" si="0"/>
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="21">
+        <v>31509</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="22">
+        <v>0</v>
+      </c>
+      <c r="K24" s="22">
+        <v>8</v>
+      </c>
+      <c r="L24">
+        <f>K24-M24</f>
+        <v>35</v>
+      </c>
+      <c r="M24" s="22">
+        <v>-27</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="22">
+        <v>80</v>
+      </c>
+      <c r="P24" s="22">
+        <v>80</v>
+      </c>
+      <c r="Q24" s="31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="21">
+        <v>24801</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K25" s="19">
+        <v>24</v>
+      </c>
+      <c r="L25">
+        <f>K25-M25</f>
+        <v>21</v>
+      </c>
+      <c r="M25" s="19">
+        <v>3</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" s="19">
+        <v>32</v>
+      </c>
+      <c r="P25" s="22">
+        <v>27</v>
+      </c>
+      <c r="Q25" s="31">
+        <f t="shared" si="0"/>
+        <v>0.33750000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="21">
+        <v>26996</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K26" s="19">
+        <v>23</v>
+      </c>
+      <c r="L26">
+        <f>K26-M26</f>
+        <v>30</v>
+      </c>
+      <c r="M26" s="19">
+        <v>-7</v>
+      </c>
+      <c r="N26" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26" s="19">
+        <v>60</v>
+      </c>
+      <c r="P26" s="22">
+        <v>68</v>
+      </c>
+      <c r="Q26" s="31">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="21">
+        <v>37050</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K27" s="19">
+        <v>26</v>
+      </c>
+      <c r="L27">
+        <f>K27-M27</f>
+        <v>29</v>
+      </c>
+      <c r="M27" s="19">
+        <v>-3</v>
+      </c>
+      <c r="N27" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O27" s="19">
+        <v>48</v>
+      </c>
+      <c r="P27" s="22">
+        <v>32</v>
+      </c>
+      <c r="Q27" s="31">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="21">
+        <v>36441</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K28" s="19">
+        <v>25</v>
+      </c>
+      <c r="L28">
+        <f>K28-M28</f>
+        <v>30</v>
+      </c>
+      <c r="M28" s="19">
+        <v>-5</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28" s="19">
+        <v>51</v>
+      </c>
+      <c r="P28" s="22">
+        <v>16</v>
+      </c>
+      <c r="Q28" s="31">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="30"/>
+      <c r="H29" s="21">
+        <v>29600</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K29" s="19">
+        <v>27</v>
+      </c>
+      <c r="L29">
+        <f>K29-M29</f>
+        <v>20</v>
+      </c>
+      <c r="M29" s="19">
+        <v>7</v>
+      </c>
+      <c r="N29" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O29" s="19">
+        <v>30</v>
+      </c>
+      <c r="P29" s="22">
+        <v>38</v>
+      </c>
+      <c r="Q29" s="31">
+        <f t="shared" si="0"/>
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="30"/>
+      <c r="H30" s="21">
+        <v>37554</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K30" s="19">
+        <v>19</v>
+      </c>
+      <c r="L30">
+        <f>K30-M30</f>
+        <v>32</v>
+      </c>
+      <c r="M30" s="19">
+        <v>-13</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O30" s="19">
+        <v>67</v>
+      </c>
+      <c r="P30" s="22">
+        <v>72</v>
+      </c>
+      <c r="Q30" s="31">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="21">
+        <v>25022</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K31" s="19">
+        <v>22</v>
+      </c>
+      <c r="L31">
+        <f>K31-M31</f>
+        <v>29</v>
+      </c>
+      <c r="M31" s="19">
+        <v>-7</v>
+      </c>
+      <c r="N31" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O31" s="19">
+        <v>61</v>
+      </c>
+      <c r="P31" s="22">
+        <v>69</v>
+      </c>
+      <c r="Q31" s="31">
+        <f t="shared" si="0"/>
+        <v>0.86250000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="21">
+        <v>37523</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K32" s="19">
+        <v>23</v>
+      </c>
+      <c r="L32">
+        <f>K32-M32</f>
+        <v>32</v>
+      </c>
+      <c r="M32" s="19">
+        <v>-9</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O32" s="19">
+        <v>63</v>
+      </c>
+      <c r="P32" s="22">
+        <v>58</v>
+      </c>
+      <c r="Q32" s="31">
+        <f t="shared" si="0"/>
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="21">
+        <v>37388</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K33" s="19">
+        <v>25</v>
+      </c>
+      <c r="L33">
+        <f>K33-M33</f>
+        <v>28</v>
+      </c>
+      <c r="M33" s="19">
+        <v>-3</v>
+      </c>
+      <c r="N33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O33" s="19">
+        <v>49</v>
+      </c>
+      <c r="P33" s="22">
+        <v>50</v>
+      </c>
+      <c r="Q33" s="31">
+        <f t="shared" si="0"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="21">
+        <v>36324</v>
+      </c>
+      <c r="I34">
+        <v>6</v>
+      </c>
+      <c r="J34" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K34" s="19">
+        <v>32</v>
+      </c>
+      <c r="L34">
+        <f>K34-M34</f>
+        <v>13</v>
+      </c>
+      <c r="M34" s="19">
+        <v>19</v>
+      </c>
+      <c r="N34" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34" s="19">
+        <v>6</v>
+      </c>
+      <c r="P34" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="31">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="30"/>
+      <c r="H35" s="21">
+        <v>35450</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K35" s="19">
+        <v>30</v>
+      </c>
+      <c r="L35">
+        <f>K35-M35</f>
+        <v>26</v>
+      </c>
+      <c r="M35" s="19">
+        <v>4</v>
+      </c>
+      <c r="N35" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" s="19">
+        <v>31</v>
+      </c>
+      <c r="P35" s="22">
+        <v>26</v>
+      </c>
+      <c r="Q35" s="31">
+        <f t="shared" si="0"/>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="30"/>
+      <c r="H36" s="21">
+        <v>37683</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36" s="22">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K36" s="22">
+        <v>28</v>
+      </c>
+      <c r="L36">
+        <f>K36-M36</f>
+        <v>29</v>
+      </c>
+      <c r="M36" s="22">
+        <v>-1</v>
+      </c>
+      <c r="N36" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="22">
+        <v>45</v>
+      </c>
+      <c r="P36" s="22">
+        <v>47</v>
+      </c>
+      <c r="Q36" s="31">
+        <f t="shared" si="0"/>
+        <v>0.58750000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="30"/>
+      <c r="H37" s="21">
+        <v>33414</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K37" s="19">
+        <v>23</v>
+      </c>
+      <c r="L37">
+        <f>K37-M37</f>
+        <v>27</v>
+      </c>
+      <c r="M37" s="19">
+        <v>-4</v>
+      </c>
+      <c r="N37" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="19">
+        <v>50</v>
+      </c>
+      <c r="P37" s="22">
+        <v>51</v>
+      </c>
+      <c r="Q37" s="31">
+        <f t="shared" si="0"/>
+        <v>0.63749999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="30"/>
+      <c r="H38" s="21">
+        <v>28784</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="J38" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K38" s="19">
+        <v>31</v>
+      </c>
+      <c r="L38">
+        <f>K38-M38</f>
+        <v>19</v>
+      </c>
+      <c r="M38" s="19">
+        <v>12</v>
+      </c>
+      <c r="N38" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" s="19">
+        <v>14</v>
+      </c>
+      <c r="P38" s="22">
+        <v>17</v>
+      </c>
+      <c r="Q38" s="31">
+        <f t="shared" si="0"/>
+        <v>0.21249999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="30"/>
+      <c r="H39" s="21">
+        <v>30053</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="J39" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K39" s="19">
+        <v>30</v>
+      </c>
+      <c r="L39">
+        <f>K39-M39</f>
+        <v>23</v>
+      </c>
+      <c r="M39" s="19">
+        <v>7</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" s="19">
+        <v>29</v>
+      </c>
+      <c r="P39" s="22">
+        <v>37</v>
+      </c>
+      <c r="Q39" s="31">
+        <f t="shared" si="0"/>
+        <v>0.46250000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="21">
+        <v>37195</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K40" s="19">
+        <v>24</v>
+      </c>
+      <c r="L40">
+        <f>K40-M40</f>
+        <v>31</v>
+      </c>
+      <c r="M40" s="19">
+        <v>-7</v>
+      </c>
+      <c r="N40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O40" s="19">
+        <v>54</v>
+      </c>
+      <c r="P40" s="22">
+        <v>65</v>
+      </c>
+      <c r="Q40" s="31">
+        <f t="shared" si="0"/>
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="30"/>
+      <c r="H41" s="21">
+        <v>37115</v>
+      </c>
+      <c r="I41">
+        <v>4</v>
+      </c>
+      <c r="J41" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K41" s="19">
+        <v>27</v>
+      </c>
+      <c r="L41">
+        <f>K41-M41</f>
+        <v>25</v>
+      </c>
+      <c r="M41" s="19">
+        <v>2</v>
+      </c>
+      <c r="N41" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O41" s="19">
+        <v>34</v>
+      </c>
+      <c r="P41" s="22">
+        <v>28</v>
+      </c>
+      <c r="Q41" s="31">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="30"/>
+      <c r="H42" s="21">
+        <v>17990</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42" s="22">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K42" s="22">
+        <v>21</v>
+      </c>
+      <c r="L42">
+        <f>K42-M42</f>
+        <v>34</v>
+      </c>
+      <c r="M42" s="22">
+        <v>-13</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="22">
+        <v>70</v>
+      </c>
+      <c r="P42" s="22">
+        <v>73</v>
+      </c>
+      <c r="Q42" s="31">
+        <f t="shared" si="0"/>
+        <v>0.91249999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="30"/>
+      <c r="H43" s="21">
+        <v>33369</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K43" s="19">
+        <v>29</v>
+      </c>
+      <c r="L43">
+        <f>K43-M43</f>
+        <v>16</v>
+      </c>
+      <c r="M43" s="19">
+        <v>13</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O43" s="19">
+        <v>13</v>
+      </c>
+      <c r="P43" s="22">
+        <v>13</v>
+      </c>
+      <c r="Q43" s="31">
+        <f t="shared" si="0"/>
+        <v>0.16250000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="30"/>
+      <c r="H44" s="21">
+        <v>34789</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K44" s="19">
+        <v>27</v>
+      </c>
+      <c r="L44">
+        <f>K44-M44</f>
+        <v>22</v>
+      </c>
+      <c r="M44" s="19">
+        <v>5</v>
+      </c>
+      <c r="N44" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O44" s="19">
+        <v>25</v>
+      </c>
+      <c r="P44" s="22">
+        <v>23</v>
+      </c>
+      <c r="Q44" s="31">
+        <f t="shared" si="0"/>
+        <v>0.28749999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="30"/>
+      <c r="H45" s="21">
+        <v>26808</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K45" s="19">
+        <v>27</v>
+      </c>
+      <c r="L45">
+        <f>K45-M45</f>
+        <v>28</v>
+      </c>
+      <c r="M45" s="19">
+        <v>-1</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O45" s="19">
+        <v>47</v>
+      </c>
+      <c r="P45" s="22">
+        <v>49</v>
+      </c>
+      <c r="Q45" s="31">
+        <f t="shared" si="0"/>
+        <v>0.61250000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="30"/>
+      <c r="H46" s="21">
+        <v>36677</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K46" s="19">
+        <v>28</v>
+      </c>
+      <c r="L46">
+        <f>K46-M46</f>
+        <v>27</v>
+      </c>
+      <c r="M46" s="19">
+        <v>1</v>
+      </c>
+      <c r="N46" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O46" s="19">
+        <v>26</v>
+      </c>
+      <c r="P46" s="22">
+        <v>36</v>
+      </c>
+      <c r="Q46" s="31">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="30"/>
+      <c r="H47" s="21">
+        <v>18372</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47" s="22">
+        <v>0</v>
+      </c>
+      <c r="K47" s="22">
+        <v>12</v>
+      </c>
+      <c r="L47">
+        <f>K47-M47</f>
+        <v>34</v>
+      </c>
+      <c r="M47" s="22">
+        <v>-22</v>
+      </c>
+      <c r="N47" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O47" s="22">
+        <v>76</v>
+      </c>
+      <c r="P47" s="22">
+        <v>76</v>
+      </c>
+      <c r="Q47" s="31">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="30"/>
+      <c r="H48" s="21">
+        <v>36047</v>
+      </c>
+      <c r="I48">
+        <v>5</v>
+      </c>
+      <c r="J48" s="22">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K48" s="22">
+        <v>33</v>
+      </c>
+      <c r="L48">
+        <f>K48-M48</f>
+        <v>23</v>
+      </c>
+      <c r="M48" s="22">
+        <v>10</v>
+      </c>
+      <c r="N48" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O48" s="22">
+        <v>17</v>
+      </c>
+      <c r="P48" s="22">
+        <v>34</v>
+      </c>
+      <c r="Q48" s="31">
+        <f t="shared" si="0"/>
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="30"/>
+      <c r="H49" s="21">
+        <v>36950</v>
+      </c>
+      <c r="I49">
+        <v>4</v>
+      </c>
+      <c r="J49" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K49" s="19">
+        <v>25</v>
+      </c>
+      <c r="L49">
+        <f>K49-M49</f>
+        <v>24</v>
+      </c>
+      <c r="M49" s="19">
+        <v>1</v>
+      </c>
+      <c r="N49" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" s="19">
+        <v>37</v>
+      </c>
+      <c r="P49" s="22">
+        <v>41</v>
+      </c>
+      <c r="Q49" s="31">
+        <f t="shared" si="0"/>
+        <v>0.51249999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="30"/>
+      <c r="H50" s="21">
+        <v>33420</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K50" s="19">
+        <v>29</v>
+      </c>
+      <c r="L50">
+        <f>K50-M50</f>
+        <v>27</v>
+      </c>
+      <c r="M50" s="19">
+        <v>2</v>
+      </c>
+      <c r="N50" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O50" s="19">
+        <v>40</v>
+      </c>
+      <c r="P50" s="22">
+        <v>43</v>
+      </c>
+      <c r="Q50" s="31">
+        <f t="shared" si="0"/>
+        <v>0.53749999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="30"/>
+      <c r="H51" s="21">
+        <v>32326</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K51" s="19">
+        <v>24</v>
+      </c>
+      <c r="L51">
+        <f>K51-M51</f>
+        <v>32</v>
+      </c>
+      <c r="M51" s="19">
+        <v>-8</v>
+      </c>
+      <c r="N51" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O51" s="19">
+        <v>57</v>
+      </c>
+      <c r="P51" s="22">
+        <v>67</v>
+      </c>
+      <c r="Q51" s="31">
+        <f t="shared" si="0"/>
+        <v>0.83750000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="30"/>
+      <c r="H52" s="21">
+        <v>36821</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K52" s="19">
+        <v>23</v>
+      </c>
+      <c r="L52">
+        <f>K52-M52</f>
+        <v>26</v>
+      </c>
+      <c r="M52" s="19">
+        <v>-3</v>
+      </c>
+      <c r="N52" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O52" s="19">
+        <v>58</v>
+      </c>
+      <c r="P52" s="22">
+        <v>55</v>
+      </c>
+      <c r="Q52" s="31">
+        <f t="shared" si="0"/>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="30"/>
+      <c r="H53" s="21">
+        <v>36782</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K53" s="19">
+        <v>29</v>
+      </c>
+      <c r="L53">
+        <f>K53-M53</f>
+        <v>20</v>
+      </c>
+      <c r="M53" s="19">
+        <v>9</v>
+      </c>
+      <c r="N53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O53" s="19">
+        <v>21</v>
+      </c>
+      <c r="P53" s="22">
+        <v>20</v>
+      </c>
+      <c r="Q53" s="31">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="30"/>
+      <c r="H54" s="21">
+        <v>32319</v>
+      </c>
+      <c r="I54">
+        <v>6</v>
+      </c>
+      <c r="J54" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K54" s="19">
+        <v>32</v>
+      </c>
+      <c r="L54">
+        <f>K54-M54</f>
+        <v>14</v>
+      </c>
+      <c r="M54" s="19">
+        <v>18</v>
+      </c>
+      <c r="N54" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O54" s="19">
+        <v>8</v>
+      </c>
+      <c r="P54" s="22">
+        <v>7</v>
+      </c>
+      <c r="Q54" s="31">
+        <f t="shared" si="0"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="30"/>
+      <c r="H55" s="21">
+        <v>33430</v>
+      </c>
+      <c r="I55">
+        <v>7</v>
+      </c>
+      <c r="J55" s="19">
+        <v>1</v>
+      </c>
+      <c r="K55" s="19">
+        <v>35</v>
+      </c>
+      <c r="L55">
+        <f>K55-M55</f>
+        <v>10</v>
+      </c>
+      <c r="M55" s="19">
+        <v>25</v>
+      </c>
+      <c r="N55" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O55" s="19">
+        <v>2</v>
+      </c>
+      <c r="P55" s="22">
+        <v>3</v>
+      </c>
+      <c r="Q55" s="31">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B56" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="30"/>
+      <c r="H56" s="21">
+        <v>31894</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K56" s="19">
+        <v>21</v>
+      </c>
+      <c r="L56">
+        <f>K56-M56</f>
+        <v>29</v>
+      </c>
+      <c r="M56" s="19">
+        <v>-8</v>
+      </c>
+      <c r="N56" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O56" s="19">
+        <v>62</v>
+      </c>
+      <c r="P56" s="22">
+        <v>57</v>
+      </c>
+      <c r="Q56" s="31">
+        <f t="shared" si="0"/>
+        <v>0.71250000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="30"/>
+      <c r="H57" s="21">
+        <v>27395</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K57" s="19">
+        <v>28</v>
+      </c>
+      <c r="L57">
+        <f>K57-M57</f>
+        <v>27</v>
+      </c>
+      <c r="M57" s="19">
+        <v>1</v>
+      </c>
+      <c r="N57" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O57" s="19">
+        <v>42</v>
+      </c>
+      <c r="P57" s="22">
+        <v>45</v>
+      </c>
+      <c r="Q57" s="31">
+        <f t="shared" si="0"/>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A58" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B58" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="30"/>
+      <c r="H58" s="21">
+        <v>35324</v>
+      </c>
+      <c r="I58">
+        <v>7</v>
+      </c>
+      <c r="J58" s="19">
+        <v>1</v>
+      </c>
+      <c r="K58" s="19">
+        <v>35</v>
+      </c>
+      <c r="L58">
+        <f>K58-M58</f>
+        <v>8</v>
+      </c>
+      <c r="M58" s="19">
+        <v>27</v>
+      </c>
+      <c r="N58" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O58" s="19">
+        <v>1</v>
+      </c>
+      <c r="P58" s="22">
+        <v>3</v>
+      </c>
+      <c r="Q58" s="31">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A59" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="30"/>
+      <c r="H59" s="21">
+        <v>25773</v>
+      </c>
+      <c r="I59">
+        <v>5</v>
+      </c>
+      <c r="J59" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K59" s="19">
+        <v>29</v>
+      </c>
+      <c r="L59">
+        <f>K59-M59</f>
+        <v>23</v>
+      </c>
+      <c r="M59" s="19">
+        <v>6</v>
+      </c>
+      <c r="N59" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O59" s="19">
+        <v>24</v>
+      </c>
+      <c r="P59" s="22">
+        <v>22</v>
+      </c>
+      <c r="Q59" s="31">
+        <f t="shared" si="0"/>
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A60" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B60" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F60" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="30"/>
+      <c r="H60" s="21">
+        <v>36061</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60" s="22">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K60" s="22">
+        <v>18</v>
+      </c>
+      <c r="L60">
+        <f>K60-M60</f>
+        <v>32</v>
+      </c>
+      <c r="M60" s="22">
+        <v>-14</v>
+      </c>
+      <c r="N60" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O60" s="22">
+        <v>68</v>
+      </c>
+      <c r="P60" s="22">
+        <v>60</v>
+      </c>
+      <c r="Q60" s="31">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A61" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="30"/>
+      <c r="H61" s="21">
+        <v>37101</v>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+      <c r="J61" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K61" s="19">
+        <v>24</v>
+      </c>
+      <c r="L61">
+        <f>K61-M61</f>
+        <v>24</v>
+      </c>
+      <c r="M61" s="19">
+        <v>0</v>
+      </c>
+      <c r="N61" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O61" s="19">
+        <v>44</v>
+      </c>
+      <c r="P61" s="22">
+        <v>46</v>
+      </c>
+      <c r="Q61" s="31">
+        <f t="shared" si="0"/>
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A62" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="30"/>
+      <c r="H62" s="21">
+        <v>37101</v>
+      </c>
+      <c r="I62">
+        <v>5</v>
+      </c>
+      <c r="J62" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K62" s="19">
+        <v>32</v>
+      </c>
+      <c r="L62">
+        <f>K62-M62</f>
+        <v>21</v>
+      </c>
+      <c r="M62" s="19">
+        <v>11</v>
+      </c>
+      <c r="N62" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O62" s="19">
+        <v>16</v>
+      </c>
+      <c r="P62" s="22">
+        <v>14</v>
+      </c>
+      <c r="Q62" s="31">
+        <f t="shared" si="0"/>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F63" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="30"/>
+      <c r="H63" s="21">
+        <v>36508</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+      <c r="J63" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K63" s="19">
+        <v>32</v>
+      </c>
+      <c r="L63">
+        <f>K63-M63</f>
+        <v>22</v>
+      </c>
+      <c r="M63" s="19">
+        <v>10</v>
+      </c>
+      <c r="N63" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O63" s="19">
+        <v>18</v>
+      </c>
+      <c r="P63" s="22">
+        <v>15</v>
+      </c>
+      <c r="Q63" s="31">
+        <f t="shared" si="0"/>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="30"/>
+      <c r="H64" s="21">
+        <v>32995</v>
+      </c>
+      <c r="I64">
+        <v>6</v>
+      </c>
+      <c r="J64" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K64" s="19">
+        <v>33</v>
+      </c>
+      <c r="L64">
+        <f>K64-M64</f>
+        <v>19</v>
+      </c>
+      <c r="M64" s="19">
+        <v>14</v>
+      </c>
+      <c r="N64" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O64" s="19">
+        <v>9</v>
+      </c>
+      <c r="P64" s="22">
+        <v>10</v>
+      </c>
+      <c r="Q64" s="31">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F65" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="30"/>
+      <c r="H65" s="21">
+        <v>35962</v>
+      </c>
+      <c r="I65">
+        <v>5</v>
+      </c>
+      <c r="J65" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K65" s="19">
+        <v>30</v>
+      </c>
+      <c r="L65">
+        <f>K65-M65</f>
+        <v>23</v>
+      </c>
+      <c r="M65" s="19">
+        <v>7</v>
+      </c>
+      <c r="N65" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O65" s="19">
+        <v>23</v>
+      </c>
+      <c r="P65" s="22">
+        <v>21</v>
+      </c>
+      <c r="Q65" s="31">
+        <f t="shared" si="0"/>
+        <v>0.26250000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F66" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="30"/>
+      <c r="H66" s="21">
+        <v>27467</v>
+      </c>
+      <c r="I66">
+        <v>4</v>
+      </c>
+      <c r="J66" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K66" s="19">
+        <v>31</v>
+      </c>
+      <c r="L66">
+        <f>K66-M66</f>
+        <v>22</v>
+      </c>
+      <c r="M66" s="19">
+        <v>9</v>
+      </c>
+      <c r="N66" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O66" s="19">
+        <v>28</v>
+      </c>
+      <c r="P66" s="22">
+        <v>25</v>
+      </c>
+      <c r="Q66" s="31">
+        <f t="shared" si="0"/>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="30"/>
+      <c r="H67" s="21">
+        <v>36128</v>
+      </c>
+      <c r="I67">
+        <v>4</v>
+      </c>
+      <c r="J67" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K67" s="19">
+        <v>27</v>
+      </c>
+      <c r="L67">
+        <f>K67-M67</f>
+        <v>25</v>
+      </c>
+      <c r="M67" s="19">
+        <v>2</v>
+      </c>
+      <c r="N67" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O67" s="19">
+        <v>34</v>
+      </c>
+      <c r="P67" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q67" s="31">
+        <f t="shared" ref="Q67:Q81" si="1">P67/MAX($P$2:$P$81)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A68" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F68" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="30"/>
+      <c r="H68" s="21">
+        <v>33784</v>
+      </c>
+      <c r="I68">
+        <v>5</v>
+      </c>
+      <c r="J68" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K68" s="19">
+        <v>32</v>
+      </c>
+      <c r="L68">
+        <f>K68-M68</f>
+        <v>23</v>
+      </c>
+      <c r="M68" s="19">
+        <v>9</v>
+      </c>
+      <c r="N68" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O68" s="19">
+        <v>20</v>
+      </c>
+      <c r="P68" s="22">
+        <v>19</v>
+      </c>
+      <c r="Q68" s="31">
+        <f t="shared" si="1"/>
+        <v>0.23749999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A69" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="30"/>
+      <c r="H69" s="21">
+        <v>26219</v>
+      </c>
+      <c r="I69">
+        <v>4</v>
+      </c>
+      <c r="J69" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K69" s="19">
+        <v>27</v>
+      </c>
+      <c r="L69">
+        <f>K69-M69</f>
+        <v>26</v>
+      </c>
+      <c r="M69" s="19">
+        <v>1</v>
+      </c>
+      <c r="N69" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O69" s="19">
+        <v>36</v>
+      </c>
+      <c r="P69" s="22">
+        <v>29</v>
+      </c>
+      <c r="Q69" s="31">
+        <f t="shared" si="1"/>
+        <v>0.36249999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A70" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F70" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="30"/>
+      <c r="H70" s="21">
+        <v>27427</v>
+      </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
+      <c r="J70" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="K70" s="19">
+        <v>31</v>
+      </c>
+      <c r="L70">
+        <f>K70-M70</f>
+        <v>19</v>
+      </c>
+      <c r="M70" s="19">
+        <v>12</v>
+      </c>
+      <c r="N70" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O70" s="19">
+        <v>14</v>
+      </c>
+      <c r="P70" s="22">
+        <v>33</v>
+      </c>
+      <c r="Q70" s="31">
+        <f t="shared" si="1"/>
+        <v>0.41249999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F71" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="30"/>
+      <c r="H71" s="21">
+        <v>28491</v>
+      </c>
+      <c r="I71">
+        <v>4</v>
+      </c>
+      <c r="J71" s="19">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="K71" s="19">
+        <v>30</v>
+      </c>
+      <c r="L71">
+        <f>K71-M71</f>
+        <v>28</v>
+      </c>
+      <c r="M71" s="19">
+        <v>2</v>
+      </c>
+      <c r="N71" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O71" s="19">
+        <v>33</v>
+      </c>
+      <c r="P71" s="22">
+        <v>39</v>
+      </c>
+      <c r="Q71" s="31">
+        <f t="shared" si="1"/>
+        <v>0.48749999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A72" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B72" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F72" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="30"/>
+      <c r="H72" s="21">
+        <v>34058</v>
+      </c>
+      <c r="I72">
+        <v>3</v>
+      </c>
+      <c r="J72" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K72" s="19">
+        <v>30</v>
+      </c>
+      <c r="L72">
+        <f>K72-M72</f>
+        <v>29</v>
+      </c>
+      <c r="M72" s="19">
+        <v>1</v>
+      </c>
+      <c r="N72" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O72" s="19">
+        <v>41</v>
+      </c>
+      <c r="P72" s="22">
+        <v>44</v>
+      </c>
+      <c r="Q72" s="31">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A73" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="30"/>
+      <c r="H73" s="21">
+        <v>30501</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73" s="22">
+        <v>0</v>
+      </c>
+      <c r="K73" s="22">
+        <v>12</v>
+      </c>
+      <c r="L73">
+        <f>K73-M73</f>
+        <v>35</v>
+      </c>
+      <c r="M73" s="22">
+        <v>-23</v>
+      </c>
+      <c r="N73" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O73" s="22">
+        <v>77</v>
+      </c>
+      <c r="P73" s="22">
+        <v>77</v>
+      </c>
+      <c r="Q73" s="31">
+        <f t="shared" si="1"/>
+        <v>0.96250000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A74" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F74" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" s="30"/>
+      <c r="H74" s="21">
+        <v>22885</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74" s="22">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K74" s="22">
+        <v>18</v>
+      </c>
+      <c r="L74">
+        <f>K74-M74</f>
+        <v>34</v>
+      </c>
+      <c r="M74" s="22">
+        <v>-16</v>
+      </c>
+      <c r="N74" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O74" s="22">
+        <v>71</v>
+      </c>
+      <c r="P74" s="22">
+        <v>74</v>
+      </c>
+      <c r="Q74" s="31">
+        <f t="shared" si="1"/>
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A75" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B75" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F75" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="30"/>
+      <c r="H75" s="21">
+        <v>36853</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75" s="22">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K75" s="22">
+        <v>16</v>
+      </c>
+      <c r="L75">
+        <f>K75-M75</f>
+        <v>33</v>
+      </c>
+      <c r="M75" s="22">
+        <v>-17</v>
+      </c>
+      <c r="N75" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O75" s="22">
+        <v>72</v>
+      </c>
+      <c r="P75" s="22">
+        <v>62</v>
+      </c>
+      <c r="Q75" s="31">
+        <f t="shared" si="1"/>
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A76" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B76" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F76" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="30"/>
+      <c r="H76" s="21">
+        <v>27167</v>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76" s="19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K76" s="19">
+        <v>18</v>
+      </c>
+      <c r="L76">
+        <f>K76-M76</f>
+        <v>30</v>
+      </c>
+      <c r="M76" s="19">
+        <v>-12</v>
+      </c>
+      <c r="N76" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O76" s="19">
+        <v>65</v>
+      </c>
+      <c r="P76" s="22">
+        <v>59</v>
+      </c>
+      <c r="Q76" s="31">
+        <f t="shared" si="1"/>
+        <v>0.73750000000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A77" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B77" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F77" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="30"/>
+      <c r="H77" s="21">
+        <v>32159</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+      <c r="K77" s="22">
+        <v>9</v>
+      </c>
+      <c r="L77">
+        <f>K77-M77</f>
+        <v>35</v>
+      </c>
+      <c r="M77" s="22">
+        <v>-26</v>
+      </c>
+      <c r="N77" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O77" s="22">
+        <v>79</v>
+      </c>
+      <c r="P77" s="22">
+        <v>79</v>
+      </c>
+      <c r="Q77" s="31">
+        <f t="shared" si="1"/>
+        <v>0.98750000000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A78" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F78" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="30"/>
+      <c r="H78" s="21">
+        <v>36875</v>
+      </c>
+      <c r="I78">
+        <v>3</v>
+      </c>
+      <c r="J78" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K78" s="19">
+        <v>21</v>
+      </c>
+      <c r="L78">
+        <f>K78-M78</f>
+        <v>28</v>
+      </c>
+      <c r="M78" s="19">
+        <v>-7</v>
+      </c>
+      <c r="N78" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O78" s="19">
+        <v>56</v>
+      </c>
+      <c r="P78" s="22">
+        <v>54</v>
+      </c>
+      <c r="Q78" s="31">
+        <f t="shared" si="1"/>
+        <v>0.67500000000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B79" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F79" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="30"/>
+      <c r="H79" s="21">
+        <v>37127</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K79" s="22">
+        <v>13</v>
+      </c>
+      <c r="L79">
+        <f>K79-M79</f>
+        <v>32</v>
+      </c>
+      <c r="M79" s="22">
+        <v>-19</v>
+      </c>
+      <c r="N79" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O79" s="22">
+        <v>73</v>
+      </c>
+      <c r="P79" s="22">
+        <v>75</v>
+      </c>
+      <c r="Q79" s="31">
+        <f t="shared" si="1"/>
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A80" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B80" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F80" t="s">
+        <v>4</v>
+      </c>
+      <c r="G80" s="30"/>
+      <c r="H80" s="21">
+        <v>36336</v>
+      </c>
+      <c r="I80">
+        <v>3</v>
+      </c>
+      <c r="J80" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K80" s="19">
+        <v>21</v>
+      </c>
+      <c r="L80">
+        <f>K80-M80</f>
+        <v>27</v>
+      </c>
+      <c r="M80" s="19">
+        <v>-6</v>
+      </c>
+      <c r="N80" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O80" s="19">
+        <v>53</v>
+      </c>
+      <c r="P80" s="22">
+        <v>53</v>
+      </c>
+      <c r="Q80" s="31">
+        <f t="shared" si="1"/>
+        <v>0.66249999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A81" s="18">
+        <v>43456</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F81" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="30"/>
+      <c r="H81" s="21">
+        <v>37109</v>
+      </c>
+      <c r="I81">
+        <v>3</v>
+      </c>
+      <c r="J81" s="19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K81" s="19">
+        <v>22</v>
+      </c>
+      <c r="L81">
+        <f>K81-M81</f>
+        <v>29</v>
+      </c>
+      <c r="M81" s="19">
+        <v>-7</v>
+      </c>
+      <c r="N81" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O81" s="19">
+        <v>55</v>
+      </c>
+      <c r="P81" s="22">
+        <v>66</v>
+      </c>
+      <c r="Q81" s="31">
+        <f t="shared" si="1"/>
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O82" s="22"/>
+      <c r="P82" s="22"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O83" s="24"/>
+      <c r="P83" s="24"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Q1" xr:uid="{168B5695-45C2-4A05-A24D-A3D77E87F1FE}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2405,12 +6736,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D419A9-B4F2-4ADD-85F0-A1275142E814}">
   <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5871,12 +10202,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602C8D9A-B729-4092-9AA8-2B568B80BAF8}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8025,7 +12356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6961ADD4-8A83-4EB5-9918-F2024588BC89}">
   <dimension ref="A1:K562"/>
   <sheetViews>
@@ -27690,12 +32021,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1442A-E3AE-4EBE-82BC-3D7AC1C3AED5}">
   <dimension ref="A1:K160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>